<commit_message>
ALU fertiggestellt und Speicheradressierungskonzept erstellt
</commit_message>
<xml_diff>
--- a/CPU V2/Speicherbereiche 16-Bit CPU.xlsx
+++ b/CPU V2/Speicherbereiche 16-Bit CPU.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Technik,Mechanik,MathematikUndInformatik\BLL Bau einer 8 Bit CPU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexd\Documents\Bau einer 8 Bit CPU\CPU V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4420A1D6-C5FE-402B-86AA-9CD0CEF3A4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65B44AE-5835-46AD-9E1E-577D50256CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5B198F4F-0DF2-4F06-A72A-621563CEDBDB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5B198F4F-0DF2-4F06-A72A-621563CEDBDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="24">
-  <si>
-    <t>Adressräume 16-Bit CPU</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="39">
   <si>
     <t>Bit No.</t>
   </si>
@@ -39,71 +36,119 @@
     <t>Bitzahl</t>
   </si>
   <si>
-    <t>Von</t>
-  </si>
-  <si>
-    <t>Bis</t>
-  </si>
-  <si>
-    <t>RAM Bereich (Programm und Daten)</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>X:</t>
   </si>
   <si>
-    <t>Don't Care</t>
-  </si>
-  <si>
     <t>U:</t>
   </si>
   <si>
-    <t>Bits used for Addressing</t>
-  </si>
-  <si>
     <t>U</t>
   </si>
   <si>
-    <t>Control Register (Konfigurationsdatenwörter)</t>
-  </si>
-  <si>
     <t>0x0000</t>
   </si>
   <si>
-    <t>0x7FFF</t>
-  </si>
-  <si>
-    <t>ROM Bereich (statische ISRs und SRs)</t>
-  </si>
-  <si>
-    <t>0xA000</t>
-  </si>
-  <si>
-    <t>0xBFFF</t>
-  </si>
-  <si>
-    <t>IO-Controller Speicherbereich</t>
-  </si>
-  <si>
-    <t>0xC000</t>
-  </si>
-  <si>
-    <t>0xDFFF</t>
-  </si>
-  <si>
-    <t>0x8000</t>
-  </si>
-  <si>
-    <t>0x9FFF</t>
+    <t>Datenspeicherbereiche der CPU</t>
+  </si>
+  <si>
+    <t>Gesamter Datenbereich (Data Space)</t>
+  </si>
+  <si>
+    <t>0xFFFF</t>
+  </si>
+  <si>
+    <t>Bemerkung</t>
+  </si>
+  <si>
+    <t>0x001F</t>
+  </si>
+  <si>
+    <t>Der gesamte Datenbereich wird über 16 Bit adressiert und besteht aus 32 Arbeitsregistern, mehreren IO-Registern und dem SRAM</t>
+  </si>
+  <si>
+    <t>Direct GPR Zugriff (5 Bit)</t>
+  </si>
+  <si>
+    <t>Für bestimmte Befehle (ALU-Befehle, …) stehen alle 32 Arbeitsregister zur Verfügung</t>
+  </si>
+  <si>
+    <t>Direct GPR Zugriff (4 Bit)</t>
+  </si>
+  <si>
+    <t>Bits used for Addressing. Are supplied via instruction</t>
+  </si>
+  <si>
+    <t>Bits to be filled from Memory Controller / Decoder</t>
+  </si>
+  <si>
+    <t>U+1</t>
+  </si>
+  <si>
+    <t>S:</t>
+  </si>
+  <si>
+    <t>Bits resulting from adding the address offset for the access mode</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Direct I/O-Register Access</t>
+  </si>
+  <si>
+    <t>0x0010</t>
+  </si>
+  <si>
+    <t>0x0060</t>
+  </si>
+  <si>
+    <t>0x005F</t>
+  </si>
+  <si>
+    <t>Für bestimmte Befehle stehen nur die Register ab r16 zur Verfügung (z.B. ldi)</t>
+  </si>
+  <si>
+    <t>Zugriff auf die 64 IO-Register über 6-Bit Adressierung in in/out</t>
+  </si>
+  <si>
+    <t>0x00FF</t>
+  </si>
+  <si>
+    <t>0x0020</t>
+  </si>
+  <si>
+    <t>Von (bzgl 16)</t>
+  </si>
+  <si>
+    <t>Bis (bzgl 16)</t>
+  </si>
+  <si>
+    <t>Zugriff auf die erweiterten 160 Spezialregister nur über lds/sts (Befehle für den gesamten Speicherbereit. Kein Extra Befehl, da nur Füller, bis SRAM). U &gt; 0x0060, sonst Zugriff auf andere Register. Wäre aber dann möglich mit in/out</t>
+  </si>
+  <si>
+    <t>U=0</t>
+  </si>
+  <si>
+    <t>0x0100</t>
+  </si>
+  <si>
+    <t>0x08FF</t>
+  </si>
+  <si>
+    <t>Zugriff auf Datenspeicher SRAM auch über 16 Bit Zugriff möglich. Offset bedenken!!</t>
+  </si>
+  <si>
+    <t>Extended I/O-Registers (&gt;0x05FF und &lt;0x0100)</t>
+  </si>
+  <si>
+    <t>SRAM (2048 Byte) (&gt;0x00FF und &lt;0x09)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,13 +180,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -214,12 +252,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
@@ -235,25 +272,24 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="Eingabe" xfId="3" builtinId="20"/>
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
-    <cellStyle name="Notiz" xfId="5" builtinId="10"/>
+    <cellStyle name="Notiz" xfId="4" builtinId="10"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Warnender Text" xfId="4" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -269,9 +305,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -309,7 +345,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -415,7 +451,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -557,7 +593,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -565,49 +601,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A884AF22-5507-4C38-AA89-1A892755D965}">
-  <dimension ref="A1:V16"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="169" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" customWidth="1"/>
-    <col min="2" max="18" width="3.7109375" customWidth="1"/>
-    <col min="19" max="19" width="45.7109375" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" customWidth="1"/>
+    <col min="2" max="18" width="3.6640625" customWidth="1"/>
+    <col min="19" max="19" width="45.6640625" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
       <c r="S1" s="3"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>16</v>
@@ -661,303 +698,432 @@
         <v>0</v>
       </c>
       <c r="S2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="U2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3">
+        <v>16</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="T4">
+        <v>5</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <v>1</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="T5">
         <v>4</v>
       </c>
-      <c r="V2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="T3">
-        <v>15</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="T4">
-        <v>13</v>
-      </c>
-      <c r="U4" s="1" t="s">
+      <c r="U5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S6" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="T5">
-        <v>13</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="S6" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="T6">
         <v>6</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="W6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="T7">
+        <v>16</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -976,12 +1142,12 @@
       <c r="R9" s="1"/>
       <c r="S9" s="4"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
-        <v>10</v>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B10" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1000,9 +1166,13 @@
       <c r="R10" s="1"/>
       <c r="S10" s="4"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1020,7 +1190,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="4"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1040,7 +1210,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="4"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1060,7 +1230,7 @@
       <c r="R13" s="1"/>
       <c r="S13" s="4"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1080,7 +1250,7 @@
       <c r="R14" s="1"/>
       <c r="S14" s="4"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1099,7 +1269,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1120,9 +1290,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:R1"/>
-    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:R1"/>
+    <mergeCell ref="T1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>